<commit_message>
what I could save before we lost it in the fire (computer crash) :(
</commit_message>
<xml_diff>
--- a/PWestSemitic-Interpolation-for-Mehri.xlsx
+++ b/PWestSemitic-Interpolation-for-Mehri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e21b893125bc2b3c/Desktop/Research/comp-sem-cfrs/Modern-South-Arabian-CFR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="937" documentId="11_F25DC773A252ABDACC10487C915A6ED05BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C88B55B-92CA-4987-BFA4-F6995EB14ED0}"/>
+  <xr:revisionPtr revIDLastSave="1044" documentId="11_F25DC773A252ABDACC10487C915A6ED05BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C552A6-457B-4105-9C6F-40CC4D623410}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="724">
   <si>
     <t>Mehri</t>
   </si>
@@ -408,9 +408,6 @@
     <t>ʔ ɨ m m</t>
   </si>
   <si>
-    <t>h aː m</t>
-  </si>
-  <si>
     <t>ʔ u m m</t>
   </si>
   <si>
@@ -750,9 +747,6 @@
     <t>uterus; pubes; lower belly</t>
   </si>
   <si>
-    <t>ħ a m t</t>
-  </si>
-  <si>
     <t>ħ o m ɛ ʃ</t>
   </si>
   <si>
@@ -915,9 +909,6 @@
     <t>ɣ a ɬ ɛː r "straw" (transl. as "g̍aśêr")</t>
   </si>
   <si>
-    <t>f e l eː ɡ "watercourse"</t>
-  </si>
-  <si>
     <t>k ɨ f l ə t "division"</t>
   </si>
   <si>
@@ -1629,9 +1620,6 @@
     <t>two</t>
   </si>
   <si>
-    <t>t r u</t>
-  </si>
-  <si>
     <t>t r e n</t>
   </si>
   <si>
@@ -2062,6 +2050,153 @@
   </si>
   <si>
     <t>z ə r ə r ə;z ə r r ə "spread in the sun to dry"</t>
+  </si>
+  <si>
+    <t>f e l eː ɡ "watercourse" (fəleːg in Bomhard)</t>
+  </si>
+  <si>
+    <t>h aː m (with ħ in other sources.)</t>
+  </si>
+  <si>
+    <t>*ʔimm-um</t>
+  </si>
+  <si>
+    <t>*ajj-um</t>
+  </si>
+  <si>
+    <t>*ʔabw-um</t>
+  </si>
+  <si>
+    <t>*ʔaχw-um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*ɣarapa? </t>
+  </si>
+  <si>
+    <t>*damara?</t>
+  </si>
+  <si>
+    <t>*tɬˀabatˀum?</t>
+  </si>
+  <si>
+    <t>*paħasa?</t>
+  </si>
+  <si>
+    <t>*paħalum</t>
+  </si>
+  <si>
+    <t>*palagum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*parasum? </t>
+  </si>
+  <si>
+    <t>*patana?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*gildum? </t>
+  </si>
+  <si>
+    <t>ħ a m t (actually ħamθ)</t>
+  </si>
+  <si>
+    <t>*ħamθ</t>
+  </si>
+  <si>
+    <t>*hajq</t>
+  </si>
+  <si>
+    <t>*χabaza</t>
+  </si>
+  <si>
+    <t>̈*χabzum</t>
+  </si>
+  <si>
+    <t>*kappum?</t>
+  </si>
+  <si>
+    <t>*kabkabum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*kalbum </t>
+  </si>
+  <si>
+    <t>*kawana</t>
+  </si>
+  <si>
+    <t>*midrum</t>
+  </si>
+  <si>
+    <t>*napaχa?</t>
+  </si>
+  <si>
+    <t>*nahaqa?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*nasaja? </t>
+  </si>
+  <si>
+    <t>*qarnum?</t>
+  </si>
+  <si>
+    <t>*ʔarnab(-at)-um</t>
+  </si>
+  <si>
+    <t>*rapaqa(-t-um?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*raħala? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*sabatˀa? </t>
+  </si>
+  <si>
+    <t>t r u (rather troːh)</t>
+  </si>
+  <si>
+    <t>̈*kasapa</t>
+  </si>
+  <si>
+    <t>*maħasa?</t>
+  </si>
+  <si>
+    <t>m a r a r a</t>
+  </si>
+  <si>
+    <t>*mawuta?</t>
+  </si>
+  <si>
+    <t>*ɬaraqum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*t͡sˀadiqum </t>
+  </si>
+  <si>
+    <t>̈*warχum</t>
+  </si>
+  <si>
+    <t>*waʕilum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*tsˀ </t>
+  </si>
+  <si>
+    <t>*ʕaːdV</t>
+  </si>
+  <si>
+    <t>*kutta:num?</t>
+  </si>
+  <si>
+    <t>*zapana?</t>
+  </si>
+  <si>
+    <t>*ðakkum?</t>
+  </si>
+  <si>
+    <t>*zamanum?</t>
+  </si>
+  <si>
+    <t>*ðanabum</t>
   </si>
 </sst>
 </file>
@@ -2105,11 +2240,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2125,6 +2259,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2392,8 +2530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2441,41 +2579,41 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2484,10 +2622,10 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>680</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -2517,35 +2655,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G4" t="s">
-        <v>133</v>
-      </c>
-      <c r="H4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" t="s">
-        <v>129</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2554,7 +2695,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2566,10 +2707,10 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" t="s">
         <v>134</v>
-      </c>
-      <c r="G5" t="s">
-        <v>135</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -2578,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K5" t="s">
         <v>8</v>
@@ -2645,7 +2786,7 @@
         <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J7" t="s">
         <v>37</v>
@@ -2689,41 +2830,41 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J9" t="s">
-        <v>138</v>
-      </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="L9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2749,35 +2890,38 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>291</v>
+      </c>
+      <c r="C11" t="s">
+        <v>718</v>
       </c>
       <c r="D11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" t="s">
         <v>140</v>
       </c>
-      <c r="E11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" t="s">
-        <v>141</v>
-      </c>
       <c r="G11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2915,17 +3059,20 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2952,23 +3099,26 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2991,1826 +3141,1937 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" t="s">
         <v>142</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>143</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>144</v>
       </c>
-      <c r="E24" t="s">
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J25" t="s">
+    </row>
+    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" t="s">
         <v>162</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" t="s">
         <v>163</v>
       </c>
-      <c r="C27" t="s">
-        <v>168</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>165</v>
       </c>
-      <c r="E27" t="s">
-        <v>164</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>166</v>
       </c>
-      <c r="G27" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28" t="s">
-        <v>296</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="J28" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" t="s">
         <v>169</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" t="s">
+        <v>309</v>
+      </c>
+      <c r="F29" t="s">
         <v>170</v>
       </c>
-      <c r="D29" t="s">
+      <c r="G29" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E29" t="s">
-        <v>312</v>
-      </c>
-      <c r="F29" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" t="s">
-        <v>172</v>
-      </c>
-      <c r="J29" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B30" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G30" t="s">
+    </row>
+    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B31" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="G31" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" t="s">
+        <v>292</v>
+      </c>
+      <c r="E32" t="s">
         <v>193</v>
-      </c>
-      <c r="B32" t="s">
-        <v>294</v>
-      </c>
-      <c r="E32" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" t="s">
         <v>188</v>
       </c>
-      <c r="B33" t="s">
-        <v>191</v>
-      </c>
-      <c r="D33" t="s">
-        <v>192</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
+        <v>185</v>
+      </c>
+      <c r="G33" t="s">
+        <v>186</v>
+      </c>
+      <c r="J33" t="s">
         <v>189</v>
       </c>
-      <c r="F33" t="s">
-        <v>186</v>
-      </c>
-      <c r="G33" t="s">
-        <v>187</v>
-      </c>
-      <c r="J33" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    </row>
+    <row r="34" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E34" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D34" t="s">
-        <v>201</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="F34" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="F34" t="s">
-        <v>198</v>
-      </c>
-      <c r="G34" t="s">
-        <v>199</v>
-      </c>
-      <c r="K34" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B35" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35" t="s">
+        <v>206</v>
+      </c>
+      <c r="E35" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" t="s">
         <v>202</v>
       </c>
-      <c r="D35" t="s">
-        <v>207</v>
-      </c>
-      <c r="E35" t="s">
-        <v>206</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>203</v>
       </c>
-      <c r="G35" t="s">
+      <c r="J35" t="s">
         <v>204</v>
-      </c>
-      <c r="J35" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>209</v>
+      </c>
+      <c r="B36" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" t="s">
+        <v>212</v>
+      </c>
+      <c r="L36" t="s">
         <v>210</v>
-      </c>
-      <c r="B36" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" t="s">
-        <v>212</v>
-      </c>
-      <c r="E36" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" t="s">
+        <v>247</v>
+      </c>
+      <c r="D37" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" t="s">
+        <v>216</v>
+      </c>
+      <c r="G37" t="s">
         <v>215</v>
       </c>
-      <c r="B37" t="s">
-        <v>249</v>
-      </c>
-      <c r="D37" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" t="s">
-        <v>218</v>
-      </c>
-      <c r="F37" t="s">
-        <v>217</v>
-      </c>
-      <c r="G37" t="s">
-        <v>216</v>
-      </c>
       <c r="H37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B38" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" t="s">
         <v>219</v>
-      </c>
-      <c r="D38" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>220</v>
+      </c>
+      <c r="B39" t="s">
+        <v>222</v>
+      </c>
+      <c r="D39" t="s">
         <v>221</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
+        <v>224</v>
+      </c>
+      <c r="F39" t="s">
         <v>223</v>
       </c>
-      <c r="D39" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>225</v>
-      </c>
-      <c r="F39" t="s">
-        <v>224</v>
-      </c>
-      <c r="G39" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B40" t="s">
         <v>227</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
+        <v>232</v>
+      </c>
+      <c r="E40" t="s">
         <v>228</v>
       </c>
-      <c r="D40" t="s">
-        <v>233</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>229</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>230</v>
       </c>
-      <c r="G40" t="s">
+      <c r="J40" t="s">
         <v>231</v>
-      </c>
-      <c r="J40" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B41" t="s">
+        <v>235</v>
+      </c>
+      <c r="D41" t="s">
+        <v>237</v>
+      </c>
+      <c r="E41" t="s">
         <v>236</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="42" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E41" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="F42" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B42" t="s">
+      <c r="J42" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D42" t="s">
-        <v>239</v>
-      </c>
-      <c r="F42" t="s">
-        <v>242</v>
-      </c>
-      <c r="J42" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B43" t="s">
+        <v>242</v>
+      </c>
+      <c r="D43" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" t="s">
+        <v>243</v>
+      </c>
+      <c r="F43" t="s">
         <v>244</v>
-      </c>
-      <c r="D43" t="s">
-        <v>247</v>
-      </c>
-      <c r="E43" t="s">
-        <v>245</v>
-      </c>
-      <c r="F43" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>251</v>
+      </c>
+      <c r="B44" t="s">
+        <v>293</v>
+      </c>
+      <c r="D44" t="s">
+        <v>250</v>
+      </c>
+      <c r="E44" t="s">
+        <v>248</v>
+      </c>
+      <c r="K44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B44" t="s">
-        <v>295</v>
-      </c>
-      <c r="D44" t="s">
-        <v>252</v>
-      </c>
-      <c r="E44" t="s">
-        <v>250</v>
-      </c>
-      <c r="K44" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="C45" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B45" t="s">
-        <v>255</v>
-      </c>
-      <c r="D45" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>255</v>
+      </c>
+      <c r="B46" t="s">
+        <v>256</v>
+      </c>
+      <c r="D46" t="s">
+        <v>258</v>
+      </c>
+      <c r="E46" t="s">
         <v>257</v>
       </c>
-      <c r="B46" t="s">
-        <v>258</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="F46" t="s">
         <v>260</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
+        <v>261</v>
+      </c>
+      <c r="H46" t="s">
         <v>259</v>
       </c>
-      <c r="F46" t="s">
+      <c r="K46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G46" t="s">
+      <c r="B47" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="H46" t="s">
-        <v>261</v>
-      </c>
-      <c r="K46" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>264</v>
-      </c>
-      <c r="B47" t="s">
-        <v>266</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="B48" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>265</v>
-      </c>
-      <c r="B48" t="s">
-        <v>267</v>
-      </c>
-      <c r="D48" t="s">
-        <v>269</v>
-      </c>
-      <c r="E48" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>269</v>
+      </c>
+      <c r="B49" t="s">
+        <v>270</v>
+      </c>
+      <c r="D49" t="s">
+        <v>272</v>
+      </c>
+      <c r="E49" t="s">
         <v>271</v>
       </c>
-      <c r="B49" t="s">
-        <v>272</v>
-      </c>
-      <c r="D49" t="s">
-        <v>274</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>273</v>
-      </c>
-      <c r="F49" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B50" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" t="s">
+        <v>275</v>
+      </c>
+      <c r="E50" t="s">
         <v>276</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>277</v>
-      </c>
-      <c r="E50" t="s">
-        <v>278</v>
-      </c>
-      <c r="F50" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
+        <v>279</v>
+      </c>
+      <c r="E51" t="s">
+        <v>280</v>
+      </c>
+      <c r="K51" t="s">
         <v>281</v>
       </c>
-      <c r="E51" t="s">
+    </row>
+    <row r="52" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="K51" t="s">
+      <c r="B52" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="C52" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D52" t="s">
-        <v>286</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="G52" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="F52" t="s">
-        <v>287</v>
-      </c>
-      <c r="G52" t="s">
-        <v>289</v>
-      </c>
-      <c r="J52" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D53" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E53" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F53" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>299</v>
+      </c>
+      <c r="B54" t="s">
+        <v>297</v>
+      </c>
+      <c r="D54" t="s">
+        <v>298</v>
+      </c>
+      <c r="E54" t="s">
+        <v>300</v>
+      </c>
+      <c r="K54" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B54" t="s">
-        <v>300</v>
-      </c>
-      <c r="D54" t="s">
-        <v>301</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="C55" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="K54" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="F55" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K55" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B55" t="s">
-        <v>305</v>
-      </c>
-      <c r="D55" t="s">
+    </row>
+    <row r="56" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="E55" t="s">
-        <v>306</v>
-      </c>
-      <c r="F55" t="s">
-        <v>308</v>
-      </c>
-      <c r="G55" t="s">
-        <v>309</v>
-      </c>
-      <c r="J55" t="s">
-        <v>310</v>
-      </c>
-      <c r="K55" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="B56" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B56" t="s">
+      <c r="F56" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D56" t="s">
+      <c r="G56" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E56" t="s">
+      <c r="J56" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="F56" t="s">
-        <v>318</v>
-      </c>
-      <c r="G56" t="s">
-        <v>319</v>
-      </c>
-      <c r="J56" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B57" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D57" t="s">
+        <v>320</v>
+      </c>
+      <c r="E57" t="s">
+        <v>322</v>
+      </c>
+      <c r="L57" t="s">
+        <v>319</v>
+      </c>
+      <c r="M57" t="s">
         <v>323</v>
-      </c>
-      <c r="E57" t="s">
-        <v>325</v>
-      </c>
-      <c r="L57" t="s">
-        <v>322</v>
-      </c>
-      <c r="M57" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>326</v>
+      </c>
+      <c r="B58" t="s">
+        <v>325</v>
+      </c>
+      <c r="D58" t="s">
+        <v>328</v>
+      </c>
+      <c r="E58" t="s">
+        <v>327</v>
+      </c>
+      <c r="F58" t="s">
+        <v>324</v>
+      </c>
+      <c r="G58" t="s">
         <v>329</v>
       </c>
-      <c r="B58" t="s">
-        <v>328</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="J58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E58" t="s">
-        <v>330</v>
-      </c>
-      <c r="F58" t="s">
-        <v>327</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="B59" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="J58" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="E59" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B59" t="s">
-        <v>336</v>
-      </c>
-      <c r="D59" t="s">
-        <v>335</v>
-      </c>
-      <c r="E59" t="s">
+    </row>
+    <row r="60" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F59" t="s">
-        <v>338</v>
-      </c>
-      <c r="J59" t="s">
+      <c r="E60" s="1" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="F60" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B60" t="s">
-        <v>343</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="J60" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="E60" t="s">
-        <v>340</v>
-      </c>
-      <c r="F60" t="s">
-        <v>346</v>
-      </c>
-      <c r="G60" t="s">
-        <v>344</v>
-      </c>
-      <c r="J60" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>345</v>
+      </c>
+      <c r="B61" t="s">
+        <v>346</v>
+      </c>
+      <c r="D61" t="s">
+        <v>344</v>
+      </c>
+      <c r="E61" t="s">
+        <v>347</v>
+      </c>
+      <c r="F61" t="s">
         <v>348</v>
       </c>
-      <c r="B61" t="s">
+      <c r="G61" t="s">
         <v>349</v>
       </c>
-      <c r="D61" t="s">
-        <v>347</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="J61" t="s">
         <v>350</v>
-      </c>
-      <c r="F61" t="s">
-        <v>351</v>
-      </c>
-      <c r="G61" t="s">
-        <v>352</v>
-      </c>
-      <c r="J61" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>351</v>
+      </c>
+      <c r="B62" t="s">
+        <v>352</v>
+      </c>
+      <c r="D62" t="s">
+        <v>357</v>
+      </c>
+      <c r="E62" t="s">
+        <v>356</v>
+      </c>
+      <c r="F62" t="s">
+        <v>353</v>
+      </c>
+      <c r="G62" t="s">
         <v>354</v>
       </c>
-      <c r="B62" t="s">
+      <c r="J62" t="s">
         <v>355</v>
-      </c>
-      <c r="D62" t="s">
-        <v>360</v>
-      </c>
-      <c r="E62" t="s">
-        <v>359</v>
-      </c>
-      <c r="F62" t="s">
-        <v>356</v>
-      </c>
-      <c r="G62" t="s">
-        <v>357</v>
-      </c>
-      <c r="J62" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>358</v>
+      </c>
+      <c r="B63" t="s">
+        <v>359</v>
+      </c>
+      <c r="D63" t="s">
+        <v>362</v>
+      </c>
+      <c r="E63" t="s">
+        <v>360</v>
+      </c>
+      <c r="J63" t="s">
         <v>361</v>
-      </c>
-      <c r="B63" t="s">
-        <v>362</v>
-      </c>
-      <c r="D63" t="s">
-        <v>365</v>
-      </c>
-      <c r="E63" t="s">
-        <v>363</v>
-      </c>
-      <c r="J63" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>363</v>
+      </c>
+      <c r="B64" t="s">
+        <v>365</v>
+      </c>
+      <c r="C64" t="s">
+        <v>699</v>
+      </c>
+      <c r="D64" t="s">
+        <v>364</v>
+      </c>
+      <c r="E64" t="s">
         <v>366</v>
       </c>
-      <c r="B64" t="s">
+      <c r="F64" t="s">
         <v>368</v>
       </c>
-      <c r="D64" t="s">
+      <c r="G64" t="s">
         <v>367</v>
       </c>
-      <c r="E64" t="s">
+      <c r="J64" t="s">
         <v>369</v>
-      </c>
-      <c r="F64" t="s">
-        <v>371</v>
-      </c>
-      <c r="G64" t="s">
-        <v>370</v>
-      </c>
-      <c r="J64" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>370</v>
+      </c>
+      <c r="B65" t="s">
+        <v>371</v>
+      </c>
+      <c r="D65" t="s">
         <v>373</v>
       </c>
-      <c r="B65" t="s">
+      <c r="E65" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D65" t="s">
+      <c r="B66" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="E65" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="E66" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="B66" t="s">
-        <v>378</v>
-      </c>
-      <c r="D66" t="s">
-        <v>379</v>
-      </c>
-      <c r="E66" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>378</v>
+      </c>
+      <c r="B67" t="s">
         <v>381</v>
       </c>
-      <c r="B67" t="s">
-        <v>384</v>
-      </c>
       <c r="D67" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E67" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>384</v>
+      </c>
+      <c r="B68" t="s">
+        <v>382</v>
+      </c>
+      <c r="D68" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B68" t="s">
-        <v>385</v>
-      </c>
-      <c r="D68" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+      <c r="F69" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="B69" t="s">
-        <v>389</v>
-      </c>
-      <c r="D69" t="s">
-        <v>393</v>
-      </c>
-      <c r="E69" t="s">
-        <v>390</v>
-      </c>
-      <c r="F69" t="s">
-        <v>392</v>
-      </c>
-      <c r="G69" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>391</v>
+      </c>
+      <c r="B70" t="s">
+        <v>392</v>
+      </c>
+      <c r="D70" t="s">
+        <v>397</v>
+      </c>
+      <c r="E70" t="s">
+        <v>396</v>
+      </c>
+      <c r="F70" t="s">
+        <v>395</v>
+      </c>
+      <c r="G70" t="s">
+        <v>393</v>
+      </c>
+      <c r="J70" t="s">
         <v>394</v>
-      </c>
-      <c r="B70" t="s">
-        <v>395</v>
-      </c>
-      <c r="D70" t="s">
-        <v>400</v>
-      </c>
-      <c r="E70" t="s">
-        <v>399</v>
-      </c>
-      <c r="F70" t="s">
-        <v>398</v>
-      </c>
-      <c r="G70" t="s">
-        <v>396</v>
-      </c>
-      <c r="J70" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>399</v>
+      </c>
+      <c r="B71" t="s">
+        <v>405</v>
+      </c>
+      <c r="D71" t="s">
+        <v>398</v>
+      </c>
+      <c r="E71" t="s">
+        <v>404</v>
+      </c>
+      <c r="F71" t="s">
+        <v>401</v>
+      </c>
+      <c r="G71" t="s">
         <v>402</v>
       </c>
-      <c r="B71" t="s">
-        <v>408</v>
-      </c>
-      <c r="D71" t="s">
-        <v>401</v>
-      </c>
-      <c r="E71" t="s">
-        <v>407</v>
-      </c>
-      <c r="F71" t="s">
-        <v>404</v>
-      </c>
-      <c r="G71" t="s">
-        <v>405</v>
-      </c>
       <c r="J71" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="L71" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>406</v>
+      </c>
+      <c r="B72" t="s">
+        <v>407</v>
+      </c>
+      <c r="D72" t="s">
+        <v>408</v>
+      </c>
+      <c r="E72" t="s">
         <v>409</v>
-      </c>
-      <c r="B72" t="s">
-        <v>410</v>
-      </c>
-      <c r="D72" t="s">
-        <v>411</v>
-      </c>
-      <c r="E72" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D73" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M73" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
+        <v>415</v>
+      </c>
+      <c r="D74" t="s">
+        <v>414</v>
+      </c>
+      <c r="E74" t="s">
+        <v>413</v>
+      </c>
+      <c r="F74" t="s">
+        <v>417</v>
+      </c>
+      <c r="G74" t="s">
         <v>418</v>
       </c>
-      <c r="D74" t="s">
-        <v>417</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="L74" t="s">
         <v>416</v>
-      </c>
-      <c r="F74" t="s">
-        <v>420</v>
-      </c>
-      <c r="G74" t="s">
-        <v>421</v>
-      </c>
-      <c r="L74" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
+        <v>419</v>
+      </c>
+      <c r="E75" t="s">
+        <v>420</v>
+      </c>
+      <c r="J75" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="E75" t="s">
+      <c r="G76" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="J75" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>428</v>
-      </c>
-      <c r="B76" t="s">
-        <v>427</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="J76" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="E76" t="s">
+      <c r="G77" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="F76" t="s">
-        <v>425</v>
-      </c>
-      <c r="G76" t="s">
-        <v>426</v>
-      </c>
-      <c r="J76" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+      <c r="J77" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C78" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="D77" t="s">
-        <v>436</v>
-      </c>
-      <c r="E77" t="s">
-        <v>432</v>
-      </c>
-      <c r="F77" t="s">
-        <v>433</v>
-      </c>
-      <c r="G77" t="s">
-        <v>434</v>
-      </c>
-      <c r="J77" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+      <c r="G78" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="K78" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="B78" t="s">
-        <v>440</v>
-      </c>
-      <c r="D78" t="s">
-        <v>446</v>
-      </c>
-      <c r="E78" t="s">
-        <v>445</v>
-      </c>
-      <c r="F78" t="s">
-        <v>442</v>
-      </c>
-      <c r="G78" t="s">
-        <v>443</v>
-      </c>
-      <c r="J78" t="s">
-        <v>444</v>
-      </c>
-      <c r="K78" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>444</v>
+      </c>
+      <c r="B79" t="s">
+        <v>445</v>
+      </c>
+      <c r="D79" t="s">
+        <v>450</v>
+      </c>
+      <c r="E79" t="s">
+        <v>446</v>
+      </c>
+      <c r="F79" t="s">
         <v>447</v>
       </c>
-      <c r="B79" t="s">
+      <c r="G79" t="s">
         <v>448</v>
       </c>
-      <c r="D79" t="s">
-        <v>453</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="J79" t="s">
         <v>449</v>
-      </c>
-      <c r="F79" t="s">
-        <v>450</v>
-      </c>
-      <c r="G79" t="s">
-        <v>451</v>
-      </c>
-      <c r="J79" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
+        <v>451</v>
+      </c>
+      <c r="D80" t="s">
+        <v>456</v>
+      </c>
+      <c r="E80" t="s">
+        <v>452</v>
+      </c>
+      <c r="F80" t="s">
+        <v>453</v>
+      </c>
+      <c r="G80" t="s">
         <v>454</v>
       </c>
-      <c r="D80" t="s">
-        <v>459</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="J80" t="s">
         <v>455</v>
-      </c>
-      <c r="F80" t="s">
-        <v>456</v>
-      </c>
-      <c r="G80" t="s">
-        <v>457</v>
-      </c>
-      <c r="J80" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
+        <v>457</v>
+      </c>
+      <c r="F81" t="s">
+        <v>458</v>
+      </c>
+      <c r="G81" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="F81" t="s">
+      <c r="B82" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="G81" t="s">
+      <c r="C82" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="L82" s="1" t="s">
         <v>462</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>463</v>
-      </c>
-      <c r="B82" t="s">
-        <v>464</v>
-      </c>
-      <c r="E82" t="s">
-        <v>469</v>
-      </c>
-      <c r="F82" t="s">
-        <v>466</v>
-      </c>
-      <c r="G82" t="s">
-        <v>467</v>
-      </c>
-      <c r="J82" t="s">
-        <v>468</v>
-      </c>
-      <c r="L82" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>467</v>
+      </c>
+      <c r="B83" t="s">
+        <v>468</v>
+      </c>
+      <c r="D83" t="s">
+        <v>471</v>
+      </c>
+      <c r="E83" t="s">
+        <v>469</v>
+      </c>
+      <c r="K83" t="s">
         <v>470</v>
-      </c>
-      <c r="B83" t="s">
-        <v>471</v>
-      </c>
-      <c r="D83" t="s">
-        <v>474</v>
-      </c>
-      <c r="E83" t="s">
-        <v>472</v>
-      </c>
-      <c r="K83" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
+        <v>472</v>
+      </c>
+      <c r="D84" t="s">
+        <v>476</v>
+      </c>
+      <c r="E84" t="s">
         <v>475</v>
       </c>
-      <c r="D84" t="s">
-        <v>479</v>
-      </c>
-      <c r="E84" t="s">
-        <v>478</v>
-      </c>
       <c r="F84" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="J84" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F85" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="K85" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>483</v>
+      </c>
+      <c r="B86" t="s">
+        <v>479</v>
+      </c>
+      <c r="D86" t="s">
+        <v>484</v>
+      </c>
+      <c r="E86" t="s">
+        <v>480</v>
+      </c>
+      <c r="F86" t="s">
+        <v>481</v>
+      </c>
+      <c r="G86" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="B86" t="s">
-        <v>482</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C87" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="E86" t="s">
-        <v>483</v>
-      </c>
-      <c r="F86" t="s">
-        <v>484</v>
-      </c>
-      <c r="G86" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+      <c r="G87" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B87" t="s">
-        <v>489</v>
-      </c>
-      <c r="D87" t="s">
+    </row>
+    <row r="88" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="E87" t="s">
-        <v>492</v>
-      </c>
-      <c r="F87" t="s">
-        <v>490</v>
-      </c>
-      <c r="G87" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>500</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="J88" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="D88" t="s">
-        <v>499</v>
-      </c>
-      <c r="E88" t="s">
-        <v>495</v>
-      </c>
-      <c r="F88" t="s">
-        <v>498</v>
-      </c>
-      <c r="G88" t="s">
-        <v>496</v>
-      </c>
-      <c r="J88" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>498</v>
+      </c>
+      <c r="B89" t="s">
+        <v>499</v>
+      </c>
+      <c r="E89" t="s">
         <v>501</v>
       </c>
-      <c r="B89" t="s">
+      <c r="G89" t="s">
         <v>502</v>
       </c>
-      <c r="E89" t="s">
+      <c r="K89" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="K89" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>506</v>
-      </c>
-      <c r="D90" t="s">
+    </row>
+    <row r="91" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="E90" t="s">
-        <v>509</v>
-      </c>
-      <c r="F90" t="s">
-        <v>507</v>
-      </c>
-      <c r="G90" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>511</v>
-      </c>
-      <c r="D91" t="s">
-        <v>512</v>
-      </c>
-      <c r="E91" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D92" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E92" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
+        <v>514</v>
+      </c>
+      <c r="D93" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E94" s="1" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
-        <v>519</v>
-      </c>
-      <c r="D94" t="s">
-        <v>520</v>
-      </c>
-      <c r="E94" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D95" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
+        <v>521</v>
+      </c>
+      <c r="D96" t="s">
+        <v>522</v>
+      </c>
+      <c r="M96" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="D96" t="s">
+      <c r="C97" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="M96" t="s">
+      <c r="E97" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B97" t="s">
+      <c r="G97" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C97" t="s">
+      <c r="J97" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="H98" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="D97" t="s">
-        <v>528</v>
-      </c>
-      <c r="F97" t="s">
-        <v>529</v>
-      </c>
-      <c r="G97" t="s">
-        <v>530</v>
-      </c>
-      <c r="J97" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+      <c r="J98" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B98" t="s">
-        <v>534</v>
-      </c>
-      <c r="D98" t="s">
-        <v>540</v>
-      </c>
-      <c r="E98" t="s">
-        <v>538</v>
-      </c>
-      <c r="F98" t="s">
-        <v>539</v>
-      </c>
-      <c r="G98" t="s">
-        <v>535</v>
-      </c>
-      <c r="H98" t="s">
-        <v>536</v>
-      </c>
-      <c r="J98" t="s">
-        <v>537</v>
-      </c>
-      <c r="M98" t="s">
-        <v>545</v>
+      <c r="M98" s="1" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B99" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D99" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="K99" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
+        <v>542</v>
+      </c>
+      <c r="D100" t="s">
+        <v>544</v>
+      </c>
+      <c r="F100" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="D100" t="s">
+      <c r="F101" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="F100" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B101" t="s">
-        <v>549</v>
-      </c>
-      <c r="D101" t="s">
+    </row>
+    <row r="102" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="E101" t="s">
-        <v>550</v>
-      </c>
-      <c r="F101" t="s">
-        <v>551</v>
-      </c>
-      <c r="G101" t="s">
+      <c r="G102" s="1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B102" t="s">
-        <v>554</v>
-      </c>
-      <c r="D102" t="s">
+    <row r="103" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="E102" t="s">
+      <c r="D103" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J103" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="F102" t="s">
-        <v>557</v>
-      </c>
-      <c r="G102" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B103" t="s">
-        <v>559</v>
-      </c>
-      <c r="D103" t="s">
-        <v>563</v>
-      </c>
-      <c r="E103" t="s">
-        <v>560</v>
-      </c>
-      <c r="F103" t="s">
-        <v>561</v>
-      </c>
-      <c r="J103" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>561</v>
+      </c>
+      <c r="B104" t="s">
+        <v>560</v>
+      </c>
+      <c r="C104" t="s">
+        <v>717</v>
+      </c>
+      <c r="D104" t="s">
+        <v>562</v>
+      </c>
+      <c r="E104" t="s">
+        <v>563</v>
+      </c>
+      <c r="F104" t="s">
+        <v>564</v>
+      </c>
+      <c r="G104" t="s">
         <v>565</v>
       </c>
-      <c r="B104" t="s">
-        <v>564</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="J104" t="s">
         <v>566</v>
       </c>
-      <c r="E104" t="s">
+    </row>
+    <row r="105" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="F104" t="s">
+      <c r="B105" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="G104" t="s">
+      <c r="C105" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="J104" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>571</v>
-      </c>
-      <c r="B105" t="s">
-        <v>572</v>
-      </c>
-      <c r="D105" t="s">
-        <v>574</v>
-      </c>
-      <c r="E105" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B106" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="D106" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E106" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="K106" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B107" t="s">
+        <v>575</v>
+      </c>
+      <c r="D107" t="s">
+        <v>581</v>
+      </c>
+      <c r="E107" t="s">
+        <v>576</v>
+      </c>
+      <c r="F107" t="s">
+        <v>578</v>
+      </c>
+      <c r="G107" t="s">
         <v>579</v>
       </c>
-      <c r="D107" t="s">
-        <v>585</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="J107" t="s">
         <v>580</v>
-      </c>
-      <c r="F107" t="s">
-        <v>582</v>
-      </c>
-      <c r="G107" t="s">
-        <v>583</v>
-      </c>
-      <c r="J107" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>583</v>
+      </c>
+      <c r="B108" t="s">
+        <v>584</v>
+      </c>
+      <c r="E108" t="s">
         <v>587</v>
       </c>
-      <c r="B108" t="s">
-        <v>588</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
+        <v>586</v>
+      </c>
+      <c r="G108" t="s">
+        <v>586</v>
+      </c>
+      <c r="J108" t="s">
         <v>591</v>
       </c>
-      <c r="F108" t="s">
-        <v>590</v>
-      </c>
-      <c r="G108" t="s">
-        <v>590</v>
-      </c>
-      <c r="J108" t="s">
-        <v>595</v>
-      </c>
       <c r="L108" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B109" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D109" t="s">
+        <v>588</v>
+      </c>
+      <c r="E109" t="s">
         <v>592</v>
-      </c>
-      <c r="E109" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="110" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>601</v>
-      </c>
       <c r="F110" s="1" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
+        <v>601</v>
+      </c>
+      <c r="D111" t="s">
+        <v>599</v>
+      </c>
+      <c r="E111" t="s">
+        <v>600</v>
+      </c>
+      <c r="K111" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="D111" t="s">
+      <c r="C112" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="E111" t="s">
-        <v>604</v>
-      </c>
-      <c r="K111" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>610</v>
-      </c>
-      <c r="B112" t="s">
+      <c r="G112" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="L112" s="1" t="s">
         <v>609</v>
-      </c>
-      <c r="D112" t="s">
-        <v>608</v>
-      </c>
-      <c r="F112" t="s">
-        <v>607</v>
-      </c>
-      <c r="G112" t="s">
-        <v>612</v>
-      </c>
-      <c r="J112" t="s">
-        <v>611</v>
-      </c>
-      <c r="L112" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D113" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E113" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>614</v>
+      </c>
+      <c r="B114" t="s">
+        <v>615</v>
+      </c>
+      <c r="D114" t="s">
+        <v>613</v>
+      </c>
+      <c r="E114" t="s">
+        <v>616</v>
+      </c>
+      <c r="F114" t="s">
+        <v>617</v>
+      </c>
+      <c r="G114" t="s">
         <v>618</v>
-      </c>
-      <c r="B114" t="s">
-        <v>619</v>
-      </c>
-      <c r="D114" t="s">
-        <v>617</v>
-      </c>
-      <c r="E114" t="s">
-        <v>620</v>
-      </c>
-      <c r="F114" t="s">
-        <v>621</v>
-      </c>
-      <c r="G114" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B115" t="s">
+        <v>622</v>
+      </c>
+      <c r="D115" t="s">
+        <v>620</v>
+      </c>
+      <c r="E115" t="s">
+        <v>619</v>
+      </c>
+      <c r="F115" t="s">
+        <v>623</v>
+      </c>
+      <c r="G115" t="s">
+        <v>624</v>
+      </c>
+      <c r="H115" t="s">
         <v>625</v>
-      </c>
-      <c r="B115" t="s">
-        <v>626</v>
-      </c>
-      <c r="D115" t="s">
-        <v>624</v>
-      </c>
-      <c r="E115" t="s">
-        <v>623</v>
-      </c>
-      <c r="F115" t="s">
-        <v>627</v>
-      </c>
-      <c r="G115" t="s">
-        <v>628</v>
-      </c>
-      <c r="H115" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>629</v>
+      </c>
+      <c r="B116" t="s">
+        <v>626</v>
+      </c>
+      <c r="D116" t="s">
+        <v>627</v>
+      </c>
+      <c r="E116" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="B116" t="s">
-        <v>630</v>
-      </c>
-      <c r="D116" t="s">
-        <v>631</v>
-      </c>
-      <c r="E116" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>634</v>
-      </c>
-      <c r="B117" t="s">
-        <v>635</v>
-      </c>
-      <c r="D117" t="s">
-        <v>636</v>
-      </c>
-      <c r="E117" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>634</v>
+      </c>
+      <c r="B118" t="s">
+        <v>635</v>
+      </c>
+      <c r="C118" t="s">
+        <v>721</v>
+      </c>
+      <c r="D118" t="s">
+        <v>636</v>
+      </c>
+      <c r="E118" t="s">
+        <v>637</v>
+      </c>
+      <c r="G118" t="s">
         <v>638</v>
       </c>
-      <c r="B118" t="s">
+    </row>
+    <row r="119" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="D118" t="s">
+      <c r="G119" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="E118" t="s">
-        <v>641</v>
-      </c>
-      <c r="G118" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="s">
+      <c r="J119" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="B119" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="E119" s="3" t="s">
+      <c r="C120" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="F119" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="J119" s="3" t="s">
+      <c r="E120" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="F120" s="1" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="s">
+      <c r="G120" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="B120" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="D120" s="3" t="s">
+      <c r="J120" s="1" t="s">
         <v>651</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>654</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>654</v>
+      </c>
+      <c r="B121" t="s">
+        <v>653</v>
+      </c>
+      <c r="D121" t="s">
+        <v>657</v>
+      </c>
+      <c r="E121" t="s">
+        <v>655</v>
+      </c>
+      <c r="F121" t="s">
         <v>658</v>
       </c>
-      <c r="B121" t="s">
-        <v>657</v>
-      </c>
-      <c r="D121" t="s">
-        <v>661</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="G121" t="s">
         <v>659</v>
       </c>
-      <c r="F121" t="s">
-        <v>662</v>
-      </c>
-      <c r="G121" t="s">
-        <v>663</v>
-      </c>
       <c r="K121" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>660</v>
+      </c>
+      <c r="B122" t="s">
+        <v>662</v>
+      </c>
+      <c r="D122" t="s">
+        <v>661</v>
+      </c>
+      <c r="E122" t="s">
+        <v>665</v>
+      </c>
+      <c r="F122" t="s">
+        <v>663</v>
+      </c>
+      <c r="G122" t="s">
         <v>664</v>
-      </c>
-      <c r="B122" t="s">
-        <v>666</v>
-      </c>
-      <c r="D122" t="s">
-        <v>665</v>
-      </c>
-      <c r="E122" t="s">
-        <v>669</v>
-      </c>
-      <c r="F122" t="s">
-        <v>667</v>
-      </c>
-      <c r="G122" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
+        <v>666</v>
+      </c>
+      <c r="E123" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B124" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="E123" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B124" t="s">
-        <v>672</v>
-      </c>
-      <c r="D124" t="s">
-        <v>675</v>
-      </c>
-      <c r="E124" t="s">
-        <v>673</v>
-      </c>
-      <c r="F124" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D125" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="L125" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>